<commit_message>
Add new project files and update logs
Added new documentation, credentials, environment, database, and test files to eurofork/prj_04. Updated log files and prompts for recent API and analytical requests. Modified various Excel and text files in eurofork and myspace directories.
</commit_message>
<xml_diff>
--- a/myspace/cosa fare.xlsx
+++ b/myspace/cosa fare.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattia.forneron\Documents\GitHub\MyWorkFolder\myspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A78724A1-11A4-4F4C-9CC3-233197BD71F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD44C9B2-E0B2-43D7-B394-3381D9671BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="3120" windowWidth="23235" windowHeight="9225" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
     <sheet name="Foglio2" sheetId="2" r:id="rId2"/>
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Foglio3!$G$1:$G$14</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -38,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="118">
   <si>
     <t>18.20/25</t>
   </si>
@@ -379,10 +382,19 @@
     <t>Offerta</t>
   </si>
   <si>
-    <t xml:space="preserve"> - (Costo PC/2)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Totale  </t>
+  </si>
+  <si>
+    <t>Sconto Pay</t>
+  </si>
+  <si>
+    <t>Finale</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Gap tra ultimo e minore</t>
   </si>
 </sst>
 </file>
@@ -479,7 +491,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -550,19 +562,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9999"/>
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFE782E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1278,7 +1308,7 @@
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="130">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1501,7 +1531,43 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1585,82 +1651,67 @@
     <xf numFmtId="0" fontId="9" fillId="10" borderId="41" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="15" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="17" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="16" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="14" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="15" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="52" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="14" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="46" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="51" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="18" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1676,6 +1727,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFE782E"/>
+      <color rgb="FFFF9900"/>
+      <color rgb="FFFFCC00"/>
       <color rgb="FFFF9999"/>
       <color rgb="FF66FF99"/>
     </mruColors>
@@ -1712,11 +1766,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1725,8 +1778,17 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="it-IT"/>
+              <a:rPr lang="en-US"/>
               <a:t>Costo Finale</a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>nel tempo</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1744,11 +1806,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -1776,41 +1837,91 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> - (Costo PC/2)</c:v>
+                  <c:v>Finale</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:trendline>
+          <c:dLbls>
             <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="it-IT"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Foglio3!$E$2:$E$8</c:f>
+              <c:f>Foglio3!$E$2:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>45920</c:v>
                 </c:pt>
@@ -1832,15 +1943,33 @@
                 <c:pt idx="6">
                   <c:v>45925</c:v>
                 </c:pt>
+                <c:pt idx="7">
+                  <c:v>45930</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45930</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45931</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45931</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45933</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45933</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Foglio3!$I$2:$I$8</c:f>
+              <c:f>Foglio3!$I$2:$I$14</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00\ "€"</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="13"/>
                 <c:pt idx="0">
                   <c:v>917.51308749999976</c:v>
                 </c:pt>
@@ -1848,32 +1977,42 @@
                   <c:v>892.04049999999995</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>615.21549999999991</c:v>
+                  <c:v>684.71549999999991</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1170.5876249999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1017.1626249999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>963.62774999999988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-C439-4FCE-BFBE-BAF85EC1A699}"/>
+              <c16:uniqueId val="{00000000-66BB-4BC3-8DEB-725B51A42EB6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="472441392"/>
-        <c:axId val="650893040"/>
+        <c:gapWidth val="315"/>
+        <c:overlap val="-40"/>
+        <c:axId val="1315102544"/>
+        <c:axId val="1413860624"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="472441392"/>
+        <c:axId val="1315102544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1885,14 +2024,8 @@
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1903,9 +2036,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1916,14 +2048,14 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="650893040"/>
+        <c:crossAx val="1413860624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="650893040"/>
+        <c:axId val="1413860624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1932,12 +2064,23 @@
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1961,9 +2104,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -1974,7 +2116,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="472441392"/>
+        <c:crossAx val="1315102544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1988,15 +2130,25 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -2064,33 +2216,46 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="213">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
@@ -2099,38 +2264,14 @@
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
+      <a:schemeClr val="lt1">
         <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2140,23 +2281,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -2164,71 +2300,131 @@
     </cs:bodyPr>
   </cs:dataLabelCallout>
   <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:round/>
       </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointLine>
   <cs:dataPointMarker>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
-    <cs:effectRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2244,21 +2440,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2268,22 +2461,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -2292,14 +2485,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2311,14 +2503,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2330,30 +2521,35 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -2363,16 +2559,29 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
@@ -2382,14 +2591,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2401,14 +2609,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2420,27 +2627,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+  <cs:plotArea3D>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -2448,9 +2654,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2460,14 +2665,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2479,12 +2683,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2493,14 +2696,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="lt1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="25400" cap="rnd">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2509,9 +2713,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2525,15 +2728,17 @@
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2542,9 +2747,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2554,14 +2758,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2571,22 +2769,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>3810</xdr:rowOff>
+      <xdr:colOff>327548</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>179630</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>8964</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:rowOff>179630</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Grafico 7">
+        <xdr:cNvPr id="2" name="Grafico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE8DE4A5-445D-3ED9-A063-4589181A6ACA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9148A6B-615F-D7E2-9A5D-66CAF906F16F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2876,17 +3074,17 @@
       <selection activeCell="E20" sqref="E20:E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2915,7 +3113,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -2947,17 +3145,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="81" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="93" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="81" t="s">
+      <c r="B3" s="93" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="80" t="s">
+      <c r="D3" s="92" t="s">
         <v>31</v>
       </c>
       <c r="F3" t="s">
@@ -2966,82 +3164,82 @@
       <c r="G3" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="82" t="s">
+      <c r="H3" s="94" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="85" t="s">
+      <c r="I3" s="97" t="s">
         <v>45</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="82" t="s">
+      <c r="K3" s="94" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="81"/>
-      <c r="B4" s="81"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="93"/>
+      <c r="B4" s="93"/>
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="H4" s="83"/>
-      <c r="I4" s="86"/>
+      <c r="D4" s="92"/>
+      <c r="H4" s="95"/>
+      <c r="I4" s="98"/>
       <c r="J4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="83"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="81"/>
-      <c r="B5" s="81"/>
+      <c r="K4" s="95"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="93"/>
+      <c r="B5" s="93"/>
       <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="80"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="86"/>
+      <c r="D5" s="92"/>
+      <c r="H5" s="95"/>
+      <c r="I5" s="98"/>
       <c r="J5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="83"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="81"/>
-      <c r="B6" s="81"/>
+      <c r="K5" s="95"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="93"/>
+      <c r="B6" s="93"/>
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="80"/>
-      <c r="H6" s="83"/>
-      <c r="I6" s="86"/>
+      <c r="D6" s="92"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="98"/>
       <c r="J6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K6" s="83"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="81"/>
-      <c r="B7" s="81"/>
+      <c r="K6" s="95"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="93"/>
+      <c r="B7" s="93"/>
       <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="80"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="87"/>
+      <c r="D7" s="92"/>
+      <c r="H7" s="96"/>
+      <c r="I7" s="99"/>
       <c r="J7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="84"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="81"/>
-      <c r="B8" s="81"/>
+      <c r="K7" s="96"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="93"/>
+      <c r="B8" s="93"/>
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="80"/>
+      <c r="D8" s="92"/>
       <c r="H8" s="1" t="s">
         <v>21</v>
       </c>
@@ -3055,13 +3253,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="81"/>
-      <c r="B9" s="81"/>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="93"/>
+      <c r="B9" s="93"/>
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="80"/>
+      <c r="D9" s="92"/>
       <c r="H9" s="1" t="s">
         <v>22</v>
       </c>
@@ -3075,13 +3273,13 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="81"/>
-      <c r="B10" s="81"/>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="93"/>
+      <c r="B10" s="93"/>
       <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="80"/>
+      <c r="D10" s="92"/>
       <c r="H10" s="2" t="s">
         <v>23</v>
       </c>
@@ -3095,7 +3293,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -3108,20 +3306,20 @@
       <c r="D11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="80" t="s">
+      <c r="H11" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="81" t="s">
+      <c r="I11" s="93" t="s">
         <v>24</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="81" t="s">
+      <c r="K11" s="93" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -3134,14 +3332,14 @@
       <c r="D12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="80"/>
-      <c r="I12" s="81"/>
+      <c r="H12" s="92"/>
+      <c r="I12" s="93"/>
       <c r="J12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K12" s="81"/>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K12" s="93"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -3167,29 +3365,29 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="80" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="92" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="93" t="s">
         <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="81" t="s">
+      <c r="D14" s="93" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="80"/>
-      <c r="B15" s="81"/>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="92"/>
+      <c r="B15" s="93"/>
       <c r="C15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="81"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D15" s="93"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -3203,24 +3401,24 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="88" t="s">
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="100" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="89"/>
-      <c r="C19" s="88" t="s">
+      <c r="B19" s="101"/>
+      <c r="C19" s="100" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="90"/>
-      <c r="E19" s="77" t="s">
+      <c r="D19" s="102"/>
+      <c r="E19" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="F19" s="78"/>
-      <c r="G19" s="78"/>
-      <c r="H19" s="79"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="F19" s="90"/>
+      <c r="G19" s="90"/>
+      <c r="H19" s="91"/>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
         <v>46</v>
       </c>
@@ -3244,7 +3442,7 @@
       </c>
       <c r="H20" s="27"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="22" t="s">
         <v>48</v>
       </c>
@@ -3271,7 +3469,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="22" t="s">
         <v>49</v>
       </c>
@@ -3298,7 +3496,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
         <v>50</v>
       </c>
@@ -3322,7 +3520,7 @@
       </c>
       <c r="H23" s="28"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="24" t="s">
         <v>52</v>
       </c>
@@ -3346,7 +3544,7 @@
       </c>
       <c r="H24" s="28"/>
     </row>
-    <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="25" t="s">
         <v>54</v>
       </c>
@@ -3370,7 +3568,7 @@
       </c>
       <c r="H25" s="28"/>
     </row>
-    <row r="26" spans="1:8" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="18" t="s">
@@ -3390,7 +3588,7 @@
       </c>
       <c r="H26" s="28"/>
     </row>
-    <row r="27" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -3409,7 +3607,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -3428,7 +3626,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -3446,7 +3644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
     <mergeCell ref="A19:B19"/>
@@ -3479,41 +3677,41 @@
       <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="91" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="103" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="93"/>
-    </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="94" t="s">
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="104"/>
+      <c r="F1" s="104"/>
+      <c r="G1" s="105"/>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="106" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="108" t="s">
         <v>69</v>
       </c>
-      <c r="C2" s="97"/>
-      <c r="D2" s="96" t="s">
+      <c r="C2" s="109"/>
+      <c r="D2" s="108" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="97"/>
-      <c r="F2" s="96" t="s">
+      <c r="E2" s="109"/>
+      <c r="F2" s="108" t="s">
         <v>71</v>
       </c>
-      <c r="G2" s="97"/>
-    </row>
-    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="95"/>
+      <c r="G2" s="109"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="107"/>
       <c r="B3" s="57" t="s">
         <v>72</v>
       </c>
@@ -3533,7 +3731,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
         <v>74</v>
       </c>
@@ -3556,7 +3754,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="46" t="s">
         <v>74</v>
       </c>
@@ -3579,7 +3777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
         <v>46</v>
       </c>
@@ -3602,7 +3800,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="60" t="s">
         <v>75</v>
       </c>
@@ -3625,7 +3823,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="61" t="s">
         <v>49</v>
       </c>
@@ -3648,7 +3846,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="39" t="s">
         <v>76</v>
       </c>
@@ -3671,72 +3869,72 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="102">
+      <c r="B10" s="114">
         <v>60</v>
       </c>
-      <c r="C10" s="102"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="102"/>
-      <c r="F10" s="102"/>
-      <c r="G10" s="103"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C10" s="114"/>
+      <c r="D10" s="114"/>
+      <c r="E10" s="114"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="115"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="100">
+      <c r="B11" s="112">
         <v>50</v>
       </c>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="100"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="101"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C11" s="112"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="112"/>
+      <c r="F11" s="112"/>
+      <c r="G11" s="113"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="100">
+      <c r="B12" s="112">
         <v>50</v>
       </c>
-      <c r="C12" s="100"/>
-      <c r="D12" s="100"/>
-      <c r="E12" s="100"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="101"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C12" s="112"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="112"/>
+      <c r="F12" s="112"/>
+      <c r="G12" s="113"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="B13" s="100">
+      <c r="B13" s="112">
         <v>20</v>
       </c>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="101"/>
-    </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="112"/>
+      <c r="D13" s="112"/>
+      <c r="E13" s="112"/>
+      <c r="F13" s="112"/>
+      <c r="G13" s="113"/>
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="B14" s="98">
+      <c r="B14" s="110">
         <v>20</v>
       </c>
-      <c r="C14" s="98"/>
-      <c r="D14" s="98"/>
-      <c r="E14" s="98"/>
-      <c r="F14" s="98"/>
-      <c r="G14" s="99"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C14" s="110"/>
+      <c r="D14" s="110"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="110"/>
+      <c r="G14" s="111"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="64" t="s">
         <v>57</v>
       </c>
@@ -3759,7 +3957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="60" t="s">
         <v>58</v>
       </c>
@@ -3782,7 +3980,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="65" t="s">
         <v>61</v>
       </c>
@@ -3805,7 +4003,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="39" t="s">
         <v>82</v>
       </c>
@@ -3849,32 +4047,31 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07AF2492-3BB5-4AC7-86BA-9F4AC6194A71}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O20" sqref="O20"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I2" activeCellId="1" sqref="G13:H14 I2:I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="4.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="7.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="4.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.42578125" style="4" customWidth="1"/>
+    <col min="15" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="67" t="s">
         <v>112</v>
       </c>
@@ -3894,13 +4091,13 @@
         <v>85</v>
       </c>
       <c r="G1" s="67" t="s">
+        <v>113</v>
+      </c>
+      <c r="H1" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="H1" s="67" t="s">
-        <v>90</v>
-      </c>
       <c r="I1" s="67" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="K1" s="67" t="s">
         <v>100</v>
@@ -3915,36 +4112,36 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="114">
+    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="120">
         <v>1</v>
       </c>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="C2" s="116">
+      <c r="C2" s="77">
         <v>1499</v>
       </c>
-      <c r="D2" s="116">
+      <c r="D2" s="77">
         <f>(C2-M2) *(1-M4)  *(1-M6)*(1-M7)</f>
         <v>944.04824999999983</v>
       </c>
-      <c r="E2" s="117">
+      <c r="E2" s="78">
         <v>45920</v>
       </c>
-      <c r="F2" s="115" t="str">
+      <c r="F2" s="76" t="str">
         <f>TEXT(M2,"€#,#0.0") &amp; "/" &amp; TEXT(M4,"0%") &amp; "/" &amp; TEXT(M5,"0%") &amp; "/" &amp; TEXT(M8,"0%")</f>
         <v>€200,00/15%/10%/5%</v>
       </c>
-      <c r="G2" s="106">
+      <c r="G2" s="123">
         <f>D2+D3</f>
         <v>965.80324999999982</v>
       </c>
-      <c r="H2" s="106">
+      <c r="H2" s="123">
         <f>G2*(1-M9)</f>
         <v>917.51308749999976</v>
       </c>
-      <c r="I2" s="106">
+      <c r="I2" s="135">
         <f>H2</f>
         <v>917.51308749999976</v>
       </c>
@@ -3957,30 +4154,32 @@
       <c r="M2" s="69">
         <v>200</v>
       </c>
-      <c r="N2" s="68"/>
-    </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="114"/>
-      <c r="B3" s="118" t="s">
+      <c r="N2" s="81">
+        <v>45930</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="120"/>
+      <c r="B3" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="C3" s="119">
+      <c r="C3" s="79">
         <v>22.9</v>
       </c>
-      <c r="D3" s="119">
+      <c r="D3" s="79">
         <f>C3*(1-M8)</f>
         <v>21.754999999999999</v>
       </c>
-      <c r="E3" s="120">
+      <c r="E3" s="80">
         <v>45920</v>
       </c>
-      <c r="F3" s="121">
+      <c r="F3" s="73">
         <f>M8</f>
         <v>0.05</v>
       </c>
-      <c r="G3" s="107"/>
-      <c r="H3" s="107"/>
-      <c r="I3" s="107"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="136"/>
       <c r="K3" s="70" t="s">
         <v>87</v>
       </c>
@@ -3994,36 +4193,36 @@
         <v>45925</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="114">
+    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="120">
         <v>2</v>
       </c>
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="76" t="s">
         <v>95</v>
       </c>
-      <c r="C4" s="116">
+      <c r="C4" s="77">
         <v>1499</v>
       </c>
-      <c r="D4" s="116">
+      <c r="D4" s="77">
         <f>(C4-M2-M3) *(1-M4)  *(1-M6)</f>
         <v>917.23500000000001</v>
       </c>
-      <c r="E4" s="117">
+      <c r="E4" s="78">
         <v>45923</v>
       </c>
-      <c r="F4" s="115" t="str">
+      <c r="F4" s="76" t="str">
         <f>TEXT(M2,"€#,#0.0") &amp; "/" &amp; TEXT(M3,"€#,#0.0") &amp; "/" &amp; TEXT(M4,"0%") &amp; "/" &amp; TEXT(M6,"0%")</f>
         <v>€200,00/€100,00/15%/10%</v>
       </c>
-      <c r="G4" s="104">
+      <c r="G4" s="121">
         <f>D4+D5</f>
         <v>938.99</v>
       </c>
-      <c r="H4" s="104">
+      <c r="H4" s="121">
         <f>G4*(1-M9)</f>
         <v>892.04049999999995</v>
       </c>
-      <c r="I4" s="104">
+      <c r="I4" s="123">
         <f>H4</f>
         <v>892.04049999999995</v>
       </c>
@@ -4040,28 +4239,28 @@
         <v>45931</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="114"/>
-      <c r="B5" s="118" t="s">
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="120"/>
+      <c r="B5" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="119">
+      <c r="C5" s="79">
         <v>22.9</v>
       </c>
-      <c r="D5" s="119">
-        <f>C5*(1-M9)</f>
+      <c r="D5" s="79">
+        <f>C5*(1-M8)</f>
         <v>21.754999999999999</v>
       </c>
-      <c r="E5" s="120">
+      <c r="E5" s="80">
         <v>45923</v>
       </c>
-      <c r="F5" s="121">
+      <c r="F5" s="73">
         <f>M8</f>
         <v>0.05</v>
       </c>
-      <c r="G5" s="105"/>
-      <c r="H5" s="105"/>
-      <c r="I5" s="105"/>
+      <c r="G5" s="122"/>
+      <c r="H5" s="122"/>
+      <c r="I5" s="124"/>
       <c r="K5" s="70" t="s">
         <v>89</v>
       </c>
@@ -4075,38 +4274,38 @@
         <v>45921</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="114">
+    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="120">
         <v>3</v>
       </c>
-      <c r="B6" s="122" t="s">
+      <c r="B6" s="68" t="s">
         <v>95</v>
       </c>
-      <c r="C6" s="123">
+      <c r="C6" s="69">
         <v>1499</v>
       </c>
-      <c r="D6" s="123">
+      <c r="D6" s="69">
         <f>(C6-M2) *(1-M4)  *(1-M6)</f>
         <v>993.7349999999999</v>
       </c>
-      <c r="E6" s="124">
+      <c r="E6" s="81">
         <v>45925</v>
       </c>
-      <c r="F6" s="122" t="str">
+      <c r="F6" s="68" t="str">
         <f>TEXT(M2,"€#,#0.0") &amp; "/" &amp; TEXT(M4,"0%") &amp; "/" &amp; TEXT(M6,"0%")</f>
         <v>€200,00/15%/10%</v>
       </c>
-      <c r="G6" s="108">
+      <c r="G6" s="118">
         <f>D6+D7+D8</f>
         <v>1015.4899999999999</v>
       </c>
-      <c r="H6" s="108">
+      <c r="H6" s="118">
         <f>G6*(1-M9)</f>
         <v>964.71549999999991</v>
       </c>
-      <c r="I6" s="111">
-        <f>H6-(C8/2)</f>
-        <v>615.21549999999991</v>
+      <c r="I6" s="126">
+        <f>H6-(280)</f>
+        <v>684.71549999999991</v>
       </c>
       <c r="K6" s="70" t="s">
         <v>91</v>
@@ -4119,28 +4318,28 @@
       </c>
       <c r="N6" s="72"/>
     </row>
-    <row r="7" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="114"/>
-      <c r="B7" s="125" t="s">
+    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="120"/>
+      <c r="B7" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="126">
+      <c r="C7" s="83">
         <v>22.9</v>
       </c>
-      <c r="D7" s="126">
+      <c r="D7" s="83">
         <f>C7*(1-M9)</f>
         <v>21.754999999999999</v>
       </c>
-      <c r="E7" s="127">
+      <c r="E7" s="84">
         <v>45925</v>
       </c>
-      <c r="F7" s="128">
+      <c r="F7" s="85">
         <f>M8</f>
         <v>0.05</v>
       </c>
-      <c r="G7" s="109"/>
-      <c r="H7" s="109"/>
-      <c r="I7" s="112"/>
+      <c r="G7" s="125"/>
+      <c r="H7" s="125"/>
+      <c r="I7" s="127"/>
       <c r="K7" s="70" t="s">
         <v>92</v>
       </c>
@@ -4154,28 +4353,28 @@
         <v>45930</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="114"/>
-      <c r="B8" s="129" t="s">
+    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="120"/>
+      <c r="B8" s="86" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="119">
+      <c r="C8" s="79">
         <v>699</v>
       </c>
-      <c r="D8" s="119">
+      <c r="D8" s="79">
         <f>C8*(1-M10)</f>
         <v>0</v>
       </c>
-      <c r="E8" s="120">
+      <c r="E8" s="80">
         <v>45925</v>
       </c>
-      <c r="F8" s="121">
+      <c r="F8" s="73">
         <f>M10</f>
         <v>1</v>
       </c>
-      <c r="G8" s="110"/>
-      <c r="H8" s="110"/>
-      <c r="I8" s="113"/>
+      <c r="G8" s="119"/>
+      <c r="H8" s="119"/>
+      <c r="I8" s="128"/>
       <c r="K8" s="70" t="s">
         <v>93</v>
       </c>
@@ -4189,7 +4388,39 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="120">
+        <v>4</v>
+      </c>
+      <c r="B9" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="77">
+        <v>1499</v>
+      </c>
+      <c r="D9" s="77">
+        <f>(C9) *(1-M4)  *(1-M8)</f>
+        <v>1210.4424999999999</v>
+      </c>
+      <c r="E9" s="78">
+        <v>45930</v>
+      </c>
+      <c r="F9" s="76" t="str">
+        <f>TEXT(M4,"0%") &amp; "/" &amp; TEXT(M8,"0%")</f>
+        <v>15%/5%</v>
+      </c>
+      <c r="G9" s="131">
+        <f>D9+D10</f>
+        <v>1232.1975</v>
+      </c>
+      <c r="H9" s="131">
+        <f>G9*(1-M9)</f>
+        <v>1170.5876249999999</v>
+      </c>
+      <c r="I9" s="131">
+        <f>H9</f>
+        <v>1170.5876249999999</v>
+      </c>
       <c r="K9" s="70" t="s">
         <v>110</v>
       </c>
@@ -4199,9 +4430,32 @@
       <c r="M9" s="74">
         <v>0.05</v>
       </c>
-      <c r="N9" s="70"/>
-    </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="N9" s="72">
+        <v>45956</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="120"/>
+      <c r="B10" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="79">
+        <v>22.9</v>
+      </c>
+      <c r="D10" s="79">
+        <f>C10*(1-M8)</f>
+        <v>21.754999999999999</v>
+      </c>
+      <c r="E10" s="80">
+        <v>45930</v>
+      </c>
+      <c r="F10" s="73">
+        <f>M8</f>
+        <v>0.05</v>
+      </c>
+      <c r="G10" s="132"/>
+      <c r="H10" s="132"/>
+      <c r="I10" s="132"/>
       <c r="K10" s="66" t="s">
         <v>111</v>
       </c>
@@ -4215,13 +4469,157 @@
         <v>45926.583333333336</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="G11" s="76"/>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="116">
+        <v>5</v>
+      </c>
+      <c r="B11" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="77">
+        <v>1499</v>
+      </c>
+      <c r="D11" s="77">
+        <f>(C11-M2) *(1-M4)  *(1-M8)</f>
+        <v>1048.9424999999999</v>
+      </c>
+      <c r="E11" s="78">
+        <v>45931</v>
+      </c>
+      <c r="F11" s="76" t="str">
+        <f>TEXT(M2,"€#,#0.0") &amp; "/" &amp; TEXT(M4,"0%") &amp; "/" &amp; TEXT(M8,"0%")</f>
+        <v>€200,00/15%/5%</v>
+      </c>
+      <c r="G11" s="129">
+        <f>D11+D12</f>
+        <v>1070.6975</v>
+      </c>
+      <c r="H11" s="129">
+        <f>G11*(1-M9)</f>
+        <v>1017.1626249999999</v>
+      </c>
+      <c r="I11" s="129">
+        <f>H11</f>
+        <v>1017.1626249999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="117"/>
+      <c r="B12" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="79">
+        <v>22.9</v>
+      </c>
+      <c r="D12" s="79">
+        <f>C12*(1-M8)</f>
+        <v>21.754999999999999</v>
+      </c>
+      <c r="E12" s="80">
+        <v>45931</v>
+      </c>
+      <c r="F12" s="73">
+        <f>M8</f>
+        <v>0.05</v>
+      </c>
+      <c r="G12" s="130"/>
+      <c r="H12" s="130"/>
+      <c r="I12" s="130"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="116">
+        <v>6</v>
+      </c>
+      <c r="B13" s="76" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="77">
+        <v>1499</v>
+      </c>
+      <c r="D13" s="77">
+        <f>(C13-M2) *(1-M4)  *(1-M6)</f>
+        <v>993.7349999999999</v>
+      </c>
+      <c r="E13" s="78">
+        <v>45933</v>
+      </c>
+      <c r="F13" s="76" t="str">
+        <f>TEXT(M2,"€#,#0.0") &amp; "/" &amp; TEXT(M4,"0%") &amp; "/" &amp; TEXT(M6,"0%")</f>
+        <v>€200,00/15%/10%</v>
+      </c>
+      <c r="G13" s="133">
+        <f>D13+D14</f>
+        <v>1014.3449999999999</v>
+      </c>
+      <c r="H13" s="133">
+        <f>G13*(1-M8)</f>
+        <v>963.62774999999988</v>
+      </c>
+      <c r="I13" s="118">
+        <f>H13</f>
+        <v>963.62774999999988</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="117"/>
+      <c r="B14" s="66" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="79">
+        <v>22.9</v>
+      </c>
+      <c r="D14" s="79">
+        <f>C14*(1-M6)</f>
+        <v>20.61</v>
+      </c>
+      <c r="E14" s="80">
+        <v>45933</v>
+      </c>
+      <c r="F14" s="73">
+        <f>M6</f>
+        <v>0.1</v>
+      </c>
+      <c r="G14" s="134"/>
+      <c r="H14" s="134"/>
+      <c r="I14" s="119"/>
+    </row>
+    <row r="19" spans="9:14" x14ac:dyDescent="0.25">
+      <c r="I19" s="87"/>
+    </row>
+    <row r="27" spans="9:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="28" spans="9:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L28" s="67" t="s">
+        <v>116</v>
+      </c>
+      <c r="N28" s="67" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="29" spans="9:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L29" s="88">
+        <f>AVERAGE(I:I)</f>
+        <v>940.94118124999977</v>
+      </c>
+      <c r="N29" s="88">
+        <f>I13-I6</f>
+        <v>278.91224999999997</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="I6:I8"/>
+  <autoFilter ref="G1:G14" xr:uid="{07AF2492-3BB5-4AC7-86BA-9F4AC6194A71}"/>
+  <mergeCells count="24">
+    <mergeCell ref="G11:G12"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="I11:I12"/>
     <mergeCell ref="I4:I5"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="G9:G10"/>
+    <mergeCell ref="H9:H10"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="H13:H14"/>
+    <mergeCell ref="I13:I14"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
@@ -4232,6 +4630,8 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="G6:G8"/>
     <mergeCell ref="H6:H8"/>
+    <mergeCell ref="I6:I8"/>
+    <mergeCell ref="A11:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>